<commit_message>
add Top - SineA out PWM
</commit_message>
<xml_diff>
--- a/Calc/Binary_calc.xlsx
+++ b/Calc/Binary_calc.xlsx
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59,13 +55,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -347,10 +346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -361,452 +360,902 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="str">
         <f>_xlfn.BASE(A1:A50,2)</f>
-        <v>110001</v>
+        <v>110010</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="str">
         <f t="shared" ref="B2:B50" si="0">_xlfn.BASE(A2:A51,2)</f>
-        <v>110111</v>
+        <v>110101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>111101</v>
+        <v>111000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1000011</v>
+        <v>111011</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1001001</v>
+        <v>111111</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1001110</v>
+        <v>1000010</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1010011</v>
+        <v>1000101</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1010111</v>
+        <v>1000111</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1011010</v>
+        <v>1001010</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1011101</v>
+        <v>1001101</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1100000</v>
+        <v>1010000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1100001</v>
+        <v>1010010</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1100010</v>
+        <v>1010101</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1100010</v>
+        <v>1010111</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1100001</v>
+        <v>1011001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1100000</v>
+        <v>1011011</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1011101</v>
+        <v>1011100</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1011010</v>
+        <v>1011110</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1010111</v>
+        <v>1011111</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1010011</v>
+        <v>1100001</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1001110</v>
+        <v>1100010</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="B22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1001001</v>
+        <v>1100011</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="B23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1000011</v>
+        <v>1100011</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>111101</v>
+        <v>1100100</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>110111</v>
+        <v>1100100</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>110001</v>
+        <v>1100100</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>101011</v>
+        <v>1100100</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>100101</v>
+        <v>1100011</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>11111</v>
+        <v>1100011</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>11001</v>
+        <v>1100010</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>10100</v>
+        <v>1100001</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1111</v>
+        <v>1100000</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1011</v>
+        <v>1011111</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1011101</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>1011100</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1011010</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1011000</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1010110</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1010011</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1010001</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1001110</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>1001100</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="B43" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1001001</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1011</v>
+        <v>1000110</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="B45" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1111</v>
+        <v>1000011</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B46" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>10100</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="B47" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>11001</v>
+        <v>111101</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="B48" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>11111</v>
+        <v>111010</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>100101</v>
+        <v>110111</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>101011</v>
+        <f>_xlfn.BASE(A50:A99,2)</f>
+        <v>110100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>48</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f t="shared" ref="B51:B100" si="1">_xlfn.BASE(A51:A100,2)</f>
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>45</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>101101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>42</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>101010</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>39</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>100111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>36</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>100100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>33</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>100001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>30</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>11110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>27</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>11011</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>24</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>22</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>10110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>19</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>10011</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>17</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>14</v>
+      </c>
+      <c r="B63" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>12</v>
+      </c>
+      <c r="B64" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>10</v>
+      </c>
+      <c r="B65" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>8</v>
+      </c>
+      <c r="B66" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>7</v>
+      </c>
+      <c r="B67" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>5</v>
+      </c>
+      <c r="B68" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>4</v>
+      </c>
+      <c r="B69" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>3</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>2</v>
+      </c>
+      <c r="B71" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>1</v>
+      </c>
+      <c r="B72" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>1</v>
+      </c>
+      <c r="B73" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>0</v>
+      </c>
+      <c r="B74" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B75" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>1</v>
+      </c>
+      <c r="B78" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>1</v>
+      </c>
+      <c r="B79" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>2</v>
+      </c>
+      <c r="B80" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>3</v>
+      </c>
+      <c r="B81" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>5</v>
+      </c>
+      <c r="B82" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>6</v>
+      </c>
+      <c r="B83" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>8</v>
+      </c>
+      <c r="B84" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>9</v>
+      </c>
+      <c r="B85" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>11</v>
+      </c>
+      <c r="B86" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>13</v>
+      </c>
+      <c r="B87" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>15</v>
+      </c>
+      <c r="B88" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>18</v>
+      </c>
+      <c r="B89" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>10010</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>20</v>
+      </c>
+      <c r="B90" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>10100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>23</v>
+      </c>
+      <c r="B91" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>10111</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>26</v>
+      </c>
+      <c r="B92" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>11010</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>29</v>
+      </c>
+      <c r="B93" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>11101</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>31</v>
+      </c>
+      <c r="B94" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>11111</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>34</v>
+      </c>
+      <c r="B95" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>100010</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>37</v>
+      </c>
+      <c r="B96" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>100101</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>41</v>
+      </c>
+      <c r="B97" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>101001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>44</v>
+      </c>
+      <c r="B98" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>101100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>47</v>
+      </c>
+      <c r="B99" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>101111</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>50</v>
+      </c>
+      <c r="B100" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>110010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>